<commit_message>
Import of settings implemented
</commit_message>
<xml_diff>
--- a/Example_Table.xlsx
+++ b/Example_Table.xlsx
@@ -2,16 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TitleBlockData" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Settings" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,8 +432,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="1" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
@@ -625,7 +623,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="24" customWidth="1" min="1" max="1"/>
+    <col width="23" customWidth="1" min="1" max="1"/>
     <col width="132" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -644,12 +642,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Use external source</t>
+          <t>UseExternalSource</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -673,7 +671,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sheet1</t>
+          <t>TitleBlockData</t>
         </is>
       </c>
     </row>
@@ -683,7 +681,11 @@
           <t>StartCell</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -693,7 +695,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -705,7 +707,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -717,7 +719,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Settings2</t>
+          <t>Settings</t>
         </is>
       </c>
     </row>
@@ -741,7 +743,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -753,7 +755,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>'DRAWING_TITLE</t>
+          <t>DRAWING_TITLE</t>
         </is>
       </c>
     </row>
@@ -799,11 +801,7 @@
           <t>MapNoSheets</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>'Number of sheets</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -813,7 +811,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -825,7 +823,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -837,7 +835,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -849,7 +847,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Export settings -> StarCell can be changed
</commit_message>
<xml_diff>
--- a/Example_Table.xlsx
+++ b/Example_Table.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TitleBlockData" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Settings" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,11 +47,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -125,7 +129,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SettingsTable_2" displayName="SettingsTable_2" ref="A1:B19" headerRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TitleBlockTable_1" displayName="TitleBlockTable_1" ref="A1:E13" headerRowCount="1">
+  <autoFilter ref="A1:E13"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Property Name"/>
+    <tableColumn id="2" name="Property Value"/>
+    <tableColumn id="3" name="Increase value"/>
+    <tableColumn id="4" name="Multiplier"/>
+    <tableColumn id="5" name="Remarks"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="SettingsTable_2" displayName="SettingsTable_2" ref="A1:B19" headerRowCount="1">
   <autoFilter ref="A1:B19"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Name"/>
@@ -424,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,180 +450,232 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="2"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="9" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Property Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Property Value</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Increase value</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Multiplier</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>AUTHOR_NAME</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Paul Ebbers</t>
         </is>
       </c>
+      <c r="C2" s="1" t="inlineStr"/>
+      <c r="D2" s="1" t="inlineStr"/>
+      <c r="E2" s="1" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>DN</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>DN</t>
         </is>
       </c>
+      <c r="C3" s="1" t="inlineStr"/>
+      <c r="D3" s="1" t="inlineStr"/>
+      <c r="E3" s="1" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>DRAWING_TITLE</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>Test object #2</t>
         </is>
       </c>
+      <c r="C4" s="1" t="inlineStr"/>
+      <c r="D4" s="1" t="inlineStr"/>
+      <c r="E4" s="1" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FC-DATE</t>
         </is>
       </c>
+      <c r="B5" s="1" t="inlineStr"/>
+      <c r="C5" s="1" t="inlineStr"/>
+      <c r="D5" s="1" t="inlineStr"/>
+      <c r="E5" s="1" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>FC-REV</t>
         </is>
       </c>
+      <c r="B6" s="1" t="inlineStr"/>
+      <c r="C6" s="1" t="inlineStr"/>
+      <c r="D6" s="1" t="inlineStr"/>
+      <c r="E6" s="1" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>FC-SC</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
+      <c r="E7" s="1" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>FC-SH</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="1" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="1" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
+      <c r="E8" s="1" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>FC-SI</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="1" t="inlineStr">
         <is>
           <t>A4</t>
         </is>
       </c>
+      <c r="C9" s="1" t="inlineStr"/>
+      <c r="D9" s="1" t="inlineStr"/>
+      <c r="E9" s="1" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>FreeCAD_DRAWING</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="1" t="inlineStr">
         <is>
           <t>FreeCAD DRAWING</t>
         </is>
       </c>
+      <c r="C10" s="1" t="inlineStr"/>
+      <c r="D10" s="1" t="inlineStr"/>
+      <c r="E10" s="1" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>PN</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>PN</t>
         </is>
       </c>
+      <c r="C11" s="1" t="inlineStr"/>
+      <c r="D11" s="1" t="inlineStr"/>
+      <c r="E11" s="1" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>SI-1</t>
         </is>
       </c>
+      <c r="B12" s="1" t="inlineStr"/>
+      <c r="C12" s="1" t="inlineStr"/>
+      <c r="D12" s="1" t="inlineStr"/>
+      <c r="E12" s="1" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>SI-3</t>
         </is>
       </c>
+      <c r="B13" s="1" t="inlineStr"/>
+      <c r="C13" s="1" t="inlineStr"/>
+      <c r="D13" s="1" t="inlineStr"/>
+      <c r="E13" s="1" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr"/>
+      <c r="B14" s="1" t="inlineStr"/>
+      <c r="C14" s="1" t="inlineStr"/>
+      <c r="D14" s="1" t="inlineStr"/>
+      <c r="E14" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -628,224 +698,228 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>UseExternalSource</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>ExternalFile</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>D:/OneDrive/Personal Files/06_Tools &amp; Software/Portable programs/FreeCAD/Macro/Mod/TechDrawTitleBlockUtility/Example_Table.xlsx</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>SheetName</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>TitleBlockData</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>StartCell</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B2</t>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>A1</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>AutoFillTitleBlock</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>ImportSettingsXL</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>SheetName_Settings</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>Settings</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>StartCell_Settings</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="1" t="inlineStr">
         <is>
           <t>A1</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>UseFileName</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="1" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>DrwNrFieldName</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>DRAWING_TITLE</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>MapLength</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="1" t="inlineStr">
         <is>
           <t>'Length_Units</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>MapAngle</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="1" t="inlineStr">
         <is>
           <t>'Angle_Units</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>MapMass</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="1" t="inlineStr">
         <is>
           <t>'Mass_Units</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>MapNoSheets</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>IncludeLength</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="1" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>IncludeAngle</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="1" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>IncludeMass</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="1" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>IncludeNoOfSheets</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="1" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -854,28 +928,28 @@
   </sheetData>
   <dataValidations count="8">
     <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation sqref="B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation sqref="B7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation sqref="B10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation sqref="B16" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation sqref="B17" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation sqref="B18" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation sqref="B19" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Toolbar added to the TechDraw workbench. Same behavior as with the toolbar in the titleblock workbench.
</commit_message>
<xml_diff>
--- a/Example_Table.xlsx
+++ b/Example_Table.xlsx
@@ -129,8 +129,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TitleBlockTable_1" displayName="TitleBlockTable_1" ref="A1:E13" headerRowCount="1">
-  <autoFilter ref="A1:E13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TitleBlockTable_1" displayName="TitleBlockTable_1" ref="A1:E17" headerRowCount="1">
+  <autoFilter ref="A1:E17"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Property Name"/>
     <tableColumn id="2" name="Property Value"/>
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
@@ -502,12 +502,12 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>DN</t>
+          <t>Angle_Units</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>DN</t>
+          <t>°</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr"/>
@@ -517,12 +517,12 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>DRAWING_TITLE</t>
+          <t>DN</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Test object #2</t>
+          <t>DN</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr"/>
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>FC-DATE</t>
+          <t>DRAWING_TITLE</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr"/>
@@ -543,7 +543,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>FC-REV</t>
+          <t>FC-DATE</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr"/>
@@ -554,73 +554,57 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>FC-SC</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+          <t>FC-REV</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr"/>
+      <c r="C7" s="1" t="inlineStr"/>
+      <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>FC-SH</t>
+          <t>FC-SC</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr"/>
+      <c r="D8" s="1" t="inlineStr"/>
       <c r="E8" s="1" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>FC-SI</t>
+          <t>FC-SH</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>A4</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FreeCAD_DRAWING</t>
+          <t>FC-SI</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>FreeCAD DRAWING</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
@@ -630,12 +614,12 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>PN</t>
+          <t>FreeCAD_DRAWING</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>PN</t>
+          <t>FreeCAD DRAWING</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
@@ -645,10 +629,14 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>SI-1</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="inlineStr"/>
+          <t>Length_Units</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>mm</t>
+        </is>
+      </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr"/>
@@ -656,20 +644,76 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>SI-3</t>
-        </is>
-      </c>
-      <c r="B13" s="1" t="inlineStr"/>
+          <t>Mass_Units</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr"/>
-      <c r="B14" s="1" t="inlineStr"/>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Number of sheets</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr"/>
       <c r="E14" s="1" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>PN</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>PN</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr"/>
+      <c r="D15" s="1" t="inlineStr"/>
+      <c r="E15" s="1" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>SI-1</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr"/>
+      <c r="C16" s="1" t="inlineStr"/>
+      <c r="D16" s="1" t="inlineStr"/>
+      <c r="E16" s="1" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>SI-3</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr"/>
+      <c r="C17" s="1" t="inlineStr"/>
+      <c r="D17" s="1" t="inlineStr"/>
+      <c r="E17" s="1" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr"/>
+      <c r="B18" s="1" t="inlineStr"/>
+      <c r="C18" s="1" t="inlineStr"/>
+      <c r="D18" s="1" t="inlineStr"/>
+      <c r="E18" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Error in reading and writing bool settings fixed. The titleblock spreadsheet in FR gets a color and font style
</commit_message>
<xml_diff>
--- a/Example_Table.xlsx
+++ b/Example_Table.xlsx
@@ -451,7 +451,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -505,11 +505,7 @@
           <t>Angle_Units</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>°</t>
-        </is>
-      </c>
+      <c r="B3" s="1" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr"/>
       <c r="D3" s="1" t="inlineStr"/>
       <c r="E3" s="1" t="inlineStr"/>
@@ -520,11 +516,7 @@
           <t>DN</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>DN</t>
-        </is>
-      </c>
+      <c r="B4" s="1" t="inlineStr"/>
       <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr"/>
       <c r="E4" s="1" t="inlineStr"/>
@@ -535,7 +527,11 @@
           <t>DRAWING_TITLE</t>
         </is>
       </c>
-      <c r="B5" s="1" t="inlineStr"/>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Test object #2</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr"/>
@@ -568,11 +564,7 @@
           <t>FC-SC</t>
         </is>
       </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
+      <c r="B8" s="1" t="inlineStr"/>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr"/>
       <c r="E8" s="1" t="inlineStr"/>
@@ -602,11 +594,7 @@
           <t>FC-SI</t>
         </is>
       </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>A4</t>
-        </is>
-      </c>
+      <c r="B10" s="1" t="inlineStr"/>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr"/>
@@ -617,11 +605,7 @@
           <t>FreeCAD_DRAWING</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>FreeCAD DRAWING</t>
-        </is>
-      </c>
+      <c r="B11" s="1" t="inlineStr"/>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr"/>
       <c r="E11" s="1" t="inlineStr"/>
@@ -632,11 +616,7 @@
           <t>Length_Units</t>
         </is>
       </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>mm</t>
-        </is>
-      </c>
+      <c r="B12" s="1" t="inlineStr"/>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr"/>
@@ -662,11 +642,7 @@
           <t>Number of sheets</t>
         </is>
       </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="B14" s="1" t="inlineStr"/>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr"/>
       <c r="E14" s="1" t="inlineStr"/>
@@ -677,11 +653,7 @@
           <t>PN</t>
         </is>
       </c>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>PN</t>
-        </is>
-      </c>
+      <c r="B15" s="1" t="inlineStr"/>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr"/>
@@ -867,7 +839,11 @@
           <t>DrwNrFieldName</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr"/>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>'DRAWING_TITLE</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -913,7 +889,7 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -925,7 +901,7 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -937,7 +913,7 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -949,7 +925,7 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Import of templates and setting a default template from examples is added. Several bugs fixed
</commit_message>
<xml_diff>
--- a/Example_Table.xlsx
+++ b/Example_Table.xlsx
@@ -129,13 +129,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TitleBlockTable_1" displayName="TitleBlockTable_1" ref="A1:E17" headerRowCount="1">
-  <autoFilter ref="A1:E17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TitleBlockTable_1" displayName="TitleBlockTable_1" ref="A1:E21" headerRowCount="1">
+  <autoFilter ref="A1:E21"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Property Name"/>
     <tableColumn id="2" name="Property Value"/>
     <tableColumn id="3" name="Increase value"/>
-    <tableColumn id="4" name="Multiplier"/>
+    <tableColumn id="4" name="Factor"/>
     <tableColumn id="5" name="Remarks"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,10 +450,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="84" customWidth="1" min="2" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -475,7 +475,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Multiplier</t>
+          <t>Factor</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -487,12 +487,12 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>AUTHOR_NAME</t>
+          <t>ANGLE UNIT</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Paul Ebbers</t>
+          <t>°</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr"/>
@@ -502,10 +502,14 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Angle_Units</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr"/>
+          <t>APPROVER_NAME</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>APPROVER NAME</t>
+        </is>
+      </c>
       <c r="C3" s="1" t="inlineStr"/>
       <c r="D3" s="1" t="inlineStr"/>
       <c r="E3" s="1" t="inlineStr"/>
@@ -513,7 +517,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>DN</t>
+          <t>AUTHOR_NAME</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr"/>
@@ -524,14 +528,10 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>DRAWING_TITLE</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>Test object #2</t>
-        </is>
-      </c>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr"/>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr"/>
@@ -539,10 +539,14 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>FC-DATE</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr"/>
+          <t>DN</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Test object #2</t>
+        </is>
+      </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr"/>
       <c r="E6" s="1" t="inlineStr"/>
@@ -550,10 +554,14 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>FC-REV</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="inlineStr"/>
+          <t>DOCUMENT_TYPE</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Mechanical assembly drawing</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
@@ -561,7 +569,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>FC-SC</t>
+          <t>LENGTH UNIT</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr"/>
@@ -572,26 +580,22 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>FC-SH</t>
+          <t>OWNER_NAME</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>FreeCAD</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FC-SI</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr"/>
@@ -602,7 +606,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FreeCAD_DRAWING</t>
+          <t>PN</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr"/>
@@ -613,10 +617,14 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Length_Units</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="inlineStr"/>
+          <t>PROJECT NAME</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Titleblock Workbench</t>
+        </is>
+      </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr"/>
@@ -624,12 +632,12 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Mass_Units</t>
+          <t>REVISION</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>kg</t>
+          <t>REV A</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
@@ -639,10 +647,14 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Number of sheets</t>
-        </is>
-      </c>
-      <c r="B14" s="1" t="inlineStr"/>
+          <t>RIGHTS</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>(R) DO NOT DUPLICATE THIS DRAWING TO THIRD PARTIES WITHOUT OWNER'S PERMISSION !</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr"/>
       <c r="E14" s="1" t="inlineStr"/>
@@ -650,10 +662,14 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>PN</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="inlineStr"/>
+          <t>ROUGHNESS</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>3.2</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr"/>
@@ -661,10 +677,14 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>SI-1</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="inlineStr"/>
+          <t>SCALE</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>M x:x</t>
+        </is>
+      </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr"/>
       <c r="E16" s="1" t="inlineStr"/>
@@ -672,20 +692,88 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>SI-3</t>
-        </is>
-      </c>
-      <c r="B17" s="1" t="inlineStr"/>
-      <c r="C17" s="1" t="inlineStr"/>
+          <t>SHEET</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D17" s="1" t="inlineStr"/>
       <c r="E17" s="1" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr"/>
-      <c r="B18" s="1" t="inlineStr"/>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>SIZE</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr"/>
       <c r="E18" s="1" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>TITLELINE-1</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr"/>
+      <c r="D19" s="1" t="inlineStr"/>
+      <c r="E19" s="1" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>TITLELINE-2</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Module name</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr"/>
+      <c r="D20" s="1" t="inlineStr"/>
+      <c r="E20" s="1" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>TOLERANCE</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>+/- ?</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr"/>
+      <c r="D21" s="1" t="inlineStr"/>
+      <c r="E21" s="1" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr"/>
+      <c r="B22" s="1" t="inlineStr"/>
+      <c r="C22" s="1" t="inlineStr"/>
+      <c r="D22" s="1" t="inlineStr"/>
+      <c r="E22" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -841,7 +929,7 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>'DRAWING_TITLE</t>
+          <t>DN</t>
         </is>
       </c>
     </row>
@@ -867,11 +955,7 @@
           <t>MapMass</t>
         </is>
       </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>'Mass_Units</t>
-        </is>
-      </c>
+      <c r="B14" s="1" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">

</xml_diff>